<commit_message>
test: spread ETFs across two institutions
</commit_message>
<xml_diff>
--- a/tests/data/actual_ali.xlsx
+++ b/tests/data/actual_ali.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Ações" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="42">
   <si>
     <t xml:space="preserve">Produto</t>
   </si>
@@ -89,6 +89,9 @@
     <t xml:space="preserve">BIEF39 - ISHARES CORE MSCI EAFE ETF                        </t>
   </si>
   <si>
+    <t xml:space="preserve">INSTITUIÇÃO1</t>
+  </si>
+  <si>
     <t xml:space="preserve">BIEF39</t>
   </si>
   <si>
@@ -96,6 +99,9 @@
   </si>
   <si>
     <t xml:space="preserve">ETF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INSTITUIÇÃO2</t>
   </si>
   <si>
     <t xml:space="preserve">Administrador</t>
@@ -277,11 +283,11 @@
   </sheetPr>
   <dimension ref="A1:L1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.8125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="74.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="29.22"/>
@@ -404,11 +410,11 @@
   </sheetPr>
   <dimension ref="A1:K1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.8125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="73.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="29.22"/>
@@ -463,22 +469,22 @@
         <v>20</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F2" s="3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G2" s="3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>18</v>
@@ -493,17 +499,51 @@
         <v>2.22</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K4" s="0" t="s">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" s="5" t="n">
+        <v>2.22</v>
+      </c>
+      <c r="K3" s="5" t="n">
+        <v>2.22</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K5" s="0" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K5" s="5" t="n">
-        <v>2.22</v>
-      </c>
-    </row>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K6" s="5" t="n">
+        <v>4.44</v>
+      </c>
+    </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -523,11 +563,11 @@
   </sheetPr>
   <dimension ref="A1:L1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="L5" activeCellId="0" sqref="L5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.8125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="69.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="42.55"/>
@@ -560,7 +600,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>6</v>
@@ -614,7 +654,7 @@
       <selection pane="topLeft" activeCell="V2" activeCellId="0" sqref="V2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.8125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="58.75"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="40.21"/>
@@ -643,22 +683,22 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>6</v>
@@ -673,19 +713,19 @@
         <v>9</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -732,7 +772,7 @@
       <selection pane="topLeft" activeCell="M4" activeCellId="0" sqref="M4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.8125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="42.55"/>
@@ -754,13 +794,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>6</v>
@@ -775,13 +815,13 @@
         <v>9</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>11</v>

</xml_diff>